<commit_message>
Restore Overwrite but no user logs yet
</commit_message>
<xml_diff>
--- a/Backup/Manual/data_backup.xlsx
+++ b/Backup/Manual/data_backup.xlsx
@@ -621,7 +621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -692,6 +692,1089 @@
       </c>
       <c r="E3" s="2" t="n">
         <v>45482.56208333333</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:uBFS5kqH6cHAIKnVr9HZKWjaf5c4aaBwzQgzeTMfnM9AOkGGEnbTeaNO3g3gfZ8ThrBPXX3zPS4JPr4QMQX/JTidRv7mqM0hACfcRmRgWmygxtqVFiOxdpCtZ1Q4mw8Uf2NWF3Jf4rC+Mq/hrwh+kA==</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45482.56212962963</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45482.56212962963</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45482.56240740741</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45482.56240740741</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45482.57136574074</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45482.57136574074</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45482.57188657407</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>45482.57188657407</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45482.6</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>45482.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45482.60024305555</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45482.60024305555</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45482.92751157407</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45482.92751157407</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45482.92756944444</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45482.92756944444</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45482.92800925926</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45482.92800925926</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45482.92826388889</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45482.92826388889</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45482.92949074074</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45482.92949074074</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45482.92952546296</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45482.92952546296</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45482.93148148148</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>45482.93148148148</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45482.93155092592</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>45482.93155092592</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45482.93203703704</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>45482.93203703704</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45482.93207175926</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>45482.93207175926</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45482.93293981482</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>45482.93293981482</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45482.93313657407</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>45482.93313657407</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>45482.93680555555</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>45482.93680555555</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>45482.93702546296</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>45482.93702546296</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>45482.93811342592</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>45482.93811342592</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>45482.93824074074</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>45482.93824074074</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45482.93923611111</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>45482.93923611111</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>45482.93930555556</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>45482.93930555556</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>45482.94104166667</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>45482.94104166667</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>45482.94114583333</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>45482.94114583333</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45482.94344907408</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>45482.94344907408</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45482.94362268518</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>45482.94362268518</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>45482.9446875</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>45482.9446875</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>45482.94583333333</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>45482.94583333333</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>45482.94712962963</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>45482.94712962963</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>45482.94723379629</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>45482.94723379629</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>45482.94753472223</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>45482.94753472223</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>45482.94770833333</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>45482.94770833333</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>45482.94822916666</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>45482.94822916666</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>45482.94829861111</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>45482.94829861111</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>45482.94902777778</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>45482.94902777778</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>45482.94914351852</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>45482.94914351852</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>45482.94984953704</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>45482.94984953704</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>45482.94994212963</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>45482.94994212963</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>45482.95493055556</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>45482.95493055556</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>45482.95545138889</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>45482.95545138889</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>45482.95664351852</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>45482.95664351852</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>45482.95706018519</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>45482.95706018519</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>45482.95734953704</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>45482.95734953704</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>45482.95780092593</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>45482.95780092593</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>45482.97925925926</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>45482.97925925926</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>45482.97934027778</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>45482.97934027778</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>45482.98368055555</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>45482.98368055555</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>45482.98399305555</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>45482.98399305555</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>45482.9843287037</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>45482.9843287037</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>45482.98539351852</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>45482.98539351852</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>45482.98569444445</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>45482.98569444445</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>45482.98583333333</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>45482.98583333333</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>45482.98895833334</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>45482.98895833334</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:qCsQPaYdKSudUSJTF4cHsQ==</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>45482.98909722222</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>45482.98909722222</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>bW3KcumFHUEs4RaypuSXXQ==:c/twMdskw/rg9o8jlKaWIw==</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>45482.99136574074</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>45482.99136574074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>